<commit_message>
did the check valid sudoku board problem
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Leetcode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77903405-EA30-41E8-80B5-F0FC1C6A073B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17C8811-8FE2-44EE-8407-BDDE279006A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Question</t>
   </si>
@@ -94,6 +94,35 @@
   </si>
   <si>
     <t>All the solusions can be found on neetcode youtube channel or its website (or in my own leetcode solutions, just search the problem in "problems" section)</t>
+  </si>
+  <si>
+    <t>36. Valid Sudoku</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Just check the conditions as given in the problem </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>using set &amp; arrayList</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, add the chars to both of them and check if their sizes are equal, if they are not equal return false, for checking the 3x3 grid of 9x9 board use 4 loop to check, outer 2 loops increment by 3 in each iter and add the vars of outer 2 loops to rows and cols respectively (inner 2 loops i&amp;j go from 0 to 2)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -443,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,6 +590,17 @@
         <v>21</v>
       </c>
     </row>
+    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Did the Longest consecutive sequence in O(n) time
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E17C8811-8FE2-44EE-8407-BDDE279006A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05552E15-61AF-4DB5-886A-4F5A55617F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Question</t>
   </si>
@@ -122,6 +122,56 @@
         <scheme val="minor"/>
       </rPr>
       <t>, add the chars to both of them and check if their sizes are equal, if they are not equal return false, for checking the 3x3 grid of 9x9 board use 4 loop to check, outer 2 loops increment by 3 in each iter and add the vars of outer 2 loops to rows and cols respectively (inner 2 loops i&amp;j go from 0 to 2)</t>
+    </r>
+  </si>
+  <si>
+    <t>128. Longest Consecutive Sequence</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We have to do this in O(n) so use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Hashset, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">first store all nums in set called "set", then in another loop iter over all the ele in "set" &amp; if (ele-1) exits in "set" skip &amp; if it doesn’t, add that ele in aother set called "startVals" this set stores the start of every seq in nums, the finally iter over startVals in 3rd loop using for-each and inside put a while loop which will run if set.contains(val+1) and inside while loop update val = val+1 since "set" constains it and so counter++,, after the end of while loop </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>check if "counter" &gt; "longetCount" if true the update "longestCount"</t>
     </r>
   </si>
 </sst>
@@ -472,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,6 +651,17 @@
         <v>24</v>
       </c>
     </row>
+    <row r="11" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Started with 2 pointers, did the 2sum prblem using 2 ptrs
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E87958B-D996-41AE-B68F-BAAE64DC1BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD7092B-B874-4EB6-923F-279817D687E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Question</t>
   </si>
@@ -174,6 +174,16 @@
   <si>
     <t>Arrays &amp; hashing</t>
   </si>
+  <si>
+    <t>2 Pointers</t>
+  </si>
+  <si>
+    <t>167. Two Sum II - Input Array Is Sorted</t>
+  </si>
+  <si>
+    <t>use 2 pointers, "firstPtr" start from 0 &amp; "lastPtr" from arr.len-1, calculate the "sum" of numbers present at these ptrs, if(sum==target) return the curr Indexs, if(sum&gt;target) decrement "lastPtr" by 1 and if (sum&lt;target) increment "firstPtr" by 1
+This only works since arr are sorted, lets say sum&lt;target so u obviously have to move the "firstPtr" to a bigger number which is to the right since arr is sorted</t>
+  </si>
 </sst>
 </file>
 
@@ -216,12 +226,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -230,16 +255,16 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -522,144 +547,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="110.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="2"/>
-    <col min="5" max="5" width="78.33203125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="21.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="110.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="78.33203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Did the container with most water problem
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6246EA3-C7B4-4B87-9336-664AF05FC689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F2CCF9-C851-4693-A6C7-1150F7EF26F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Question</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>First sort the array to use 2 pointers then use 2 loops, since x+y+z=0 in outer for loop fix the value of "x" now in the inner loop u have 2sum-II problem traverse the array after x using "up" &amp; "down" and add the x+up+down==0 elements to "ans" list, also here check if the curr ans is == previous ans in "ans" List. In the outer for loop check condition if(curr x==prev x) then skip iter caz if curr x = prev x then we will get the same answers as prev x (IMP! Be sure to check  if(curr x==prev x) in outer for loop other whise the condition insize the while loop to check if curr ans = prev ans in "ans" list) wont work</t>
+  </si>
+  <si>
+    <t>11. Container With Most Water</t>
+  </si>
+  <si>
+    <t>This solution has 2 pointer &amp; has sort of greedy approach. Start with "up" at last position &amp; "down" pointer at indx 0. Calculate the volume by (up-down)*min(height[up], height[down]) and update the ans if its smaller. Now if "up" is at lets say height = 7 , while down is at height = 1 why would u update the ptr "up" to go to a unknown height, insead update the ptr that points to a smaller height in this example "down" ptr. If(height of down &lt; height of up) update down,, else update up,,, edge case if both heights are = it doesnt matter which u update</t>
   </si>
 </sst>
 </file>
@@ -553,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C15" sqref="C14:C15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,6 +721,17 @@
         <v>31</v>
       </c>
     </row>
+    <row r="14" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
did the trap rainwater problem
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F2CCF9-C851-4693-A6C7-1150F7EF26F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E544A88-AB6C-4572-861D-C649BAB8FD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Question</t>
   </si>
@@ -196,6 +196,13 @@
   <si>
     <t>This solution has 2 pointer &amp; has sort of greedy approach. Start with "up" at last position &amp; "down" pointer at indx 0. Calculate the volume by (up-down)*min(height[up], height[down]) and update the ans if its smaller. Now if "up" is at lets say height = 7 , while down is at height = 1 why would u update the ptr "up" to go to a unknown height, insead update the ptr that points to a smaller height in this example "down" ptr. If(height of down &lt; height of up) update down,, else update up,,, edge case if both heights are = it doesnt matter which u update</t>
   </si>
+  <si>
+    <t>42. Trapping Rain Water</t>
+  </si>
+  <si>
+    <t>The idea is to use 2 ptrs, "leftWall" &amp; "rightWall", use a while loop, inside call a func findRightWall(), this function finds the right wall give and arr &amp; leftWall, the right wall is such that It is &gt;= left wall, but incase there is no such wall in subarr leftWall to end, then return the biggest wall from subarr leftwall to end of arr.... next is a func getWaterBetween Walls() given an height arr, leftWall &amp; rightWall, it returns the am of water that can be collected between them, use a while loop &amp; initalize tmpPtr = leftWall+1, in while(tmpPtr&lt;rightWall) loop do totalWater += height[tmpPtr] - minWallHeight where minWallHeight = min(height[leftWall],height[rightWall]), then tmpPter++
+Finally after calling both these funcs change the right wall to left wall ie leftWall = rightWall,,,, now in next iter we will find right wall again</t>
+  </si>
 </sst>
 </file>
 
@@ -218,7 +225,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +241,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -277,6 +290,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -559,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,6 +748,17 @@
         <v>33</v>
       </c>
     </row>
+    <row r="15" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Did 3. Longest Substring Without Repeating Characters
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E544A88-AB6C-4572-861D-C649BAB8FD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30039380-B1B1-444F-B249-880A6401EE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Question</t>
   </si>
@@ -202,6 +202,38 @@
   <si>
     <t>The idea is to use 2 ptrs, "leftWall" &amp; "rightWall", use a while loop, inside call a func findRightWall(), this function finds the right wall give and arr &amp; leftWall, the right wall is such that It is &gt;= left wall, but incase there is no such wall in subarr leftWall to end, then return the biggest wall from subarr leftwall to end of arr.... next is a func getWaterBetween Walls() given an height arr, leftWall &amp; rightWall, it returns the am of water that can be collected between them, use a while loop &amp; initalize tmpPtr = leftWall+1, in while(tmpPtr&lt;rightWall) loop do totalWater += height[tmpPtr] - minWallHeight where minWallHeight = min(height[leftWall],height[rightWall]), then tmpPter++
 Finally after calling both these funcs change the right wall to left wall ie leftWall = rightWall,,,, now in next iter we will find right wall again</t>
+  </si>
+  <si>
+    <t>Sliding Window</t>
+  </si>
+  <si>
+    <t>3. Longest Substring Without Repeating Characters</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The idea is to use a hashset &amp; keep track of the start of the window using "winStart", iter over the chars in array, if currChar isnt present in hs then add it, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>before this</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> put a while(hs.contains(currChar)) loop do hs.remove( charArr[winstart] ) then winStart++, since we are sliding the window to the right if we detect a char same as currChar in hashset</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -575,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,6 +791,17 @@
         <v>35</v>
       </c>
     </row>
+    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
did the Min stack
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30039380-B1B1-444F-B249-880A6401EE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90394C6-DFC6-4203-9B02-43063A8D8EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>Question</t>
   </si>
@@ -234,6 +234,15 @@
       </rPr>
       <t xml:space="preserve"> put a while(hs.contains(currChar)) loop do hs.remove( charArr[winstart] ) then winStart++, since we are sliding the window to the right if we detect a char same as currChar in hashset</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Stack </t>
+  </si>
+  <si>
+    <t>155. Min Stack</t>
+  </si>
+  <si>
+    <t>We have to design a stack with operations push(), pop(), top() &amp; getMin(), all having time O(1),,, the first 3 are straightforward, but for getMin() brute force is O(n),, for getMin we will make a stack&lt;Node&gt; where node has int num (curr num) &amp; int min (this is the minimum num from curr num to end/bottom of the stack) , while pushing you set Node.num = inputNum &amp; Node.min = min(inputNum, getMin()),, ie u set min = min(input, previous minimum in stack)</t>
   </si>
 </sst>
 </file>
@@ -607,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E19" sqref="E17:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -802,6 +811,17 @@
         <v>38</v>
       </c>
     </row>
+    <row r="17" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Did the 22. Generate Parentheses question
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90394C6-DFC6-4203-9B02-43063A8D8EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18238AD-EA96-4588-817B-8240D94ACB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>Question</t>
   </si>
@@ -243,6 +243,21 @@
   </si>
   <si>
     <t>We have to design a stack with operations push(), pop(), top() &amp; getMin(), all having time O(1),,, the first 3 are straightforward, but for getMin() brute force is O(n),, for getMin we will make a stack&lt;Node&gt; where node has int num (curr num) &amp; int min (this is the minimum num from curr num to end/bottom of the stack) , while pushing you set Node.num = inputNum &amp; Node.min = min(inputNum, getMin()),, ie u set min = min(input, previous minimum in stack)</t>
+  </si>
+  <si>
+    <t>150. Evaluate Reverse Polish Notation</t>
+  </si>
+  <si>
+    <t>Use stack ,iter over tokens, put all the number inside the stack, when u encounter a operator (*,-,+,/) pop 2 nums as num1, num2 and do the specified operations on it and push the result back into the stack,, continue iterating over tokens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backtracking </t>
+  </si>
+  <si>
+    <t>22. Generate Parentheses</t>
+  </si>
+  <si>
+    <t>Do a recursive backtracking. U can add "(" if num of openParenthes&lt;n,, U can add ")" to str if num of closing parantheses &lt; num of open Parentheses,, Base case is when open Parentheses = closing Parenthses = n (num of partheses which we can use to genrate valid permutation, this is given)</t>
   </si>
 </sst>
 </file>
@@ -616,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E19" sqref="E17:E19"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,6 +837,28 @@
         <v>41</v>
       </c>
     </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
did the 739. Daily Temperatures
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18238AD-EA96-4588-817B-8240D94ACB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B07FD52-E18B-42CD-8676-DBCD585679AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>Question</t>
   </si>
@@ -258,6 +258,35 @@
   </si>
   <si>
     <t>Do a recursive backtracking. U can add "(" if num of openParenthes&lt;n,, U can add ")" to str if num of closing parantheses &lt; num of open Parentheses,, Base case is when open Parentheses = closing Parenthses = n (num of partheses which we can use to genrate valid permutation, this is given)</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>739. Daily Temperatures</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">This qs requires the understanding of monotonic stack! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Make a stack&lt;Node&gt;, Node is a class that stores tempreature value &amp; its indx, Use a for loop to iter over the array of temps. Inside put a while(stack not empty &amp; stack.top &lt; curr temp) do -&gt; stack.pop(), ans[i] = curr temp indx - popped value indx; when this is over do stack.push(new Node(currTemp, itsIndx));</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -631,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -859,6 +888,17 @@
         <v>46</v>
       </c>
     </row>
+    <row r="20" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Did the 853. Car Fleet
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69476D4F-6345-451C-A42B-5E6B662A8B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF426E08-A2E8-4A38-930B-7A09E83EE1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>Question</t>
   </si>
@@ -291,13 +291,108 @@
   <si>
     <t>Monotonic Stack link: 
 https://youtu.be/J7Ll0I-GSwA?si=DxuogRf_PFGVbM3E</t>
+  </si>
+  <si>
+    <t>Stack &amp; Math</t>
+  </si>
+  <si>
+    <t>853. Car Fleet</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Pr6T-3yB9RM?si=wIJ8hfr__GLOv1ps</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">You need to know monotonic stack!!! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">First sort both the arrs BUT only accourding to position. After sorting use stack&lt;Car&gt; &amp; iterate the position arr in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reverse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> order, define "ttt" (time to arriave on target) = (target - currCarsPosition)/currCarSpeed,,, if the curr car's ttt &lt; st.top().ttt ie curr car will arrive at target before the car on its right which is impossible in a single lane no overtaking road (given) (and since we are iter sorted position in reverse order) so curr car will slow down to the st.top() car's speed, so </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>discard</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>curr car</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. If we encounter a car with ttt &gt; st.top(), push it onto the stack... After the iter the answer = st.size()</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +404,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -364,10 +467,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -384,8 +488,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -664,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E5" sqref="E3:E5"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -893,7 +1001,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
@@ -907,8 +1015,25 @@
         <v>50</v>
       </c>
     </row>
+    <row r="21" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D21" r:id="rId1" xr:uid="{35299F42-C228-43E2-B954-EFB9EDC93588}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Did the 84. Largest Rectangle in Histogram
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF426E08-A2E8-4A38-930B-7A09E83EE1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D032A87D-9F56-4003-B6B3-F5744678F679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>Question</t>
   </si>
@@ -385,6 +385,46 @@
         <scheme val="minor"/>
       </rPr>
       <t>. If we encounter a car with ttt &gt; st.top(), push it onto the stack... After the iter the answer = st.size()</t>
+    </r>
+  </si>
+  <si>
+    <t>84. Largest Rectangle in Histogram</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">U need to understand monotonic stack first!!!,,,, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This solution is too hard for me to explain watch this video for visual explaination:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://youtu.be/zx5Sw9130L0?si=79lWeV1xHcdTWbPt</t>
     </r>
   </si>
 </sst>
@@ -772,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1029,6 +1069,17 @@
         <v>53</v>
       </c>
     </row>
+    <row r="22" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D21" r:id="rId1" xr:uid="{35299F42-C228-43E2-B954-EFB9EDC93588}"/>

</xml_diff>

<commit_message>
Did 74. Search a 2D Matrix
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D032A87D-9F56-4003-B6B3-F5744678F679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D570BC2D-1381-440C-9106-F3CF687E7A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t>Question</t>
   </si>
@@ -426,6 +426,19 @@
       </rPr>
       <t>https://youtu.be/zx5Sw9130L0?si=79lWeV1xHcdTWbPt</t>
     </r>
+  </si>
+  <si>
+    <t>This Apprach use the usual binary seach. 
+First check if the target &lt; mat[0][0] or target &gt; mat[end][end] if true return false
+First you search the rows to see in which row the target lies, do this using binary search! 
+Then after finding the row use normal binary search on the potential row in which the target lies, if found return true
+after all this if the func is still going that means target does not exist in the mat, return false</t>
+  </si>
+  <si>
+    <t>74. Search a 2D Matrix</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
   </si>
 </sst>
 </file>
@@ -812,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1080,6 +1093,17 @@
         <v>56</v>
       </c>
     </row>
+    <row r="23" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D21" r:id="rId1" xr:uid="{35299F42-C228-43E2-B954-EFB9EDC93588}"/>

</xml_diff>

<commit_message>
did 875. Koko Eating Bananas
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D570BC2D-1381-440C-9106-F3CF687E7A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6A9D1D-8E3C-43F7-AC8C-37D12DC1F4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
   <si>
     <t>Question</t>
   </si>
@@ -439,6 +439,23 @@
   </si>
   <si>
     <t>Binary Search</t>
+  </si>
+  <si>
+    <t>875. Koko Eating Bananas</t>
+  </si>
+  <si>
+    <t>Do binary search ON "k" dont sort any piles or anything
+kstart =1, kend = max(piles)
+use while loop (kstart&lt;=kend){
+kmid = middle of kstart and kend
+calculate timeTaken with kmid
+if(timeTake&lt;=h) { //we are taking less than expected time, so we can further decrease speed of eating
+	k = min(k, kmid)
+	kend = kmid -1
+}
+else { //we are taking more than expected time, so increase speed of eating
+k start = kmid+1
+}</t>
   </si>
 </sst>
 </file>
@@ -825,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1104,6 +1121,17 @@
         <v>57</v>
       </c>
     </row>
+    <row r="24" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D21" r:id="rId1" xr:uid="{35299F42-C228-43E2-B954-EFB9EDC93588}"/>

</xml_diff>

<commit_message>
Did 224. Basic Calculator , BUT MY APPROACH IS VERY INEFFICIENT
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6A9D1D-8E3C-43F7-AC8C-37D12DC1F4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB62CCB1-767A-4014-BD0A-47A2D2A4CF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
   <si>
     <t>Question</t>
   </si>
@@ -456,6 +456,21 @@
 else { //we are taking more than expected time, so increase speed of eating
 k start = kmid+1
 }</t>
+  </si>
+  <si>
+    <t>Stack &amp; Recursion</t>
+  </si>
+  <si>
+    <t>224. Basic Calculator</t>
+  </si>
+  <si>
+    <t>first convert to postfix, in postfix put "," before everytime u encounter a operator to indicate end of a number
+then in soultution everytime u encounter a single "," parse the final number u made from chars to Integer and store in stack
+if u encounter 2 ",," simultaneously that means there was a a expression like 1 -(-2) which means u should push a 0 to the stack when u encounter a ",,"
+if u encounter ,2,3+ in postfix this means the expression was "-2+3", in postfix we add "," evertime we encounter a operator to indicate end of num, since there was no num before "-" this means that the "-" is unary operator, so push a 0 here too!</t>
+  </si>
+  <si>
+    <t>My approach is very inefficent, checkout a efficient approach on YT or Leetcode</t>
   </si>
 </sst>
 </file>
@@ -541,7 +556,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -559,6 +574,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -842,10 +860,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1132,6 +1150,20 @@
         <v>61</v>
       </c>
     </row>
+    <row r="25" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D21" r:id="rId1" xr:uid="{35299F42-C228-43E2-B954-EFB9EDC93588}"/>

</xml_diff>

<commit_message>
did the Minimum in Rotated Sorted Array - Binary Search - Leetcode 153
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB62CCB1-767A-4014-BD0A-47A2D2A4CF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B499EE2-54D8-40FA-96EC-0F2975107B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
   <si>
     <t>Question</t>
   </si>
@@ -471,6 +471,24 @@
   </si>
   <si>
     <t>My approach is very inefficent, checkout a efficient approach on YT or Leetcode</t>
+  </si>
+  <si>
+    <t>153. Find Minimum in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">couldnt solve on my own, solution by inomag,
+The main idea is, the element is said to be minimum in the rotated sorted array if the previous element to it is greater than it or there is no previous element(i.e. no rotation). We can do this using Binary search
+Find the mid element i.e. mid = (low+high)/2
+If the (mid+1)th element is less than mid element then return (mid+1)th element
+If the mid element is less than (mid-1)th element then return the mid element
+If the last element is greater than mid element then search in left half
+If the last element is less than mid element then search in right half
+Basically we are checking if we are currently in the left sorted portion (the rotated portion) or the right sorted portion. We always want to search "right" sorted portion caz all vals in right sorted portion are garanteed to be &lt; vals in left sorted portion in the subarr caz of the rotation
+</t>
+  </si>
+  <si>
+    <t>https://youtu.be/nIVW4P8b1VA?si=5Y_vMEutgdF12nqb
+https://youtu.be/nhEMDKMB44g?si=whOJgZL9QywEWoZn</t>
   </si>
 </sst>
 </file>
@@ -556,7 +574,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -574,9 +592,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -860,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1154,7 +1169,7 @@
       <c r="A25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="5" t="s">
         <v>63</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1162,13 +1177,28 @@
       </c>
       <c r="D25" s="4" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D21" r:id="rId1" xr:uid="{35299F42-C228-43E2-B954-EFB9EDC93588}"/>
+    <hyperlink ref="D26" r:id="rId2" display="https://youtu.be/nIVW4P8b1VA?si=5Y_vMEutgdF12nqb" xr:uid="{FA4BDA58-B1DD-48D8-9C29-B4B1FADE61A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
did the 33. Search in Rotated Sorted Array
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B499EE2-54D8-40FA-96EC-0F2975107B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7538DB01-9318-4289-AD58-AC18650502B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
   <si>
     <t>Question</t>
   </si>
@@ -489,6 +489,13 @@
   <si>
     <t>https://youtu.be/nIVW4P8b1VA?si=5Y_vMEutgdF12nqb
 https://youtu.be/nhEMDKMB44g?si=whOJgZL9QywEWoZn</t>
+  </si>
+  <si>
+    <t>33. Search in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>for this question u need to know problem - Minimum in Rotated Sorted Array - Binary Search - Leetcode 153
+the minimum in rotated array is nothing but the border/pivot element in rotated arr, so once u get its indx u can do simple binary search on the 2 subarray arrays divided by pivot</t>
   </si>
 </sst>
 </file>
@@ -875,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1193,6 +1200,17 @@
         <v>68</v>
       </c>
     </row>
+    <row r="27" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D21" r:id="rId1" xr:uid="{35299F42-C228-43E2-B954-EFB9EDC93588}"/>

</xml_diff>

<commit_message>
did 4. Median of Two Sorted Arrays (Extremly hard)
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C494BB2-D66C-4589-804C-1F0D6B92F9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854B04B9-4154-4C78-8194-55914F745AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
   <si>
     <t>Question</t>
   </si>
@@ -509,6 +509,15 @@
   </si>
   <si>
     <t>Binary Search &amp; Hashing</t>
+  </si>
+  <si>
+    <t>This question is EXTREMELY HARD refer to neetcodes video for explaination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://youtu.be/q6IEA26hvXc?si=RB1SByCLUSeiK4li </t>
+  </si>
+  <si>
+    <t>4. Median of Two Sorted Arrays</t>
   </si>
 </sst>
 </file>
@@ -895,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1235,12 +1244,27 @@
         <v>71</v>
       </c>
     </row>
+    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D21" r:id="rId1" xr:uid="{35299F42-C228-43E2-B954-EFB9EDC93588}"/>
     <hyperlink ref="D26" r:id="rId2" display="https://youtu.be/nIVW4P8b1VA?si=5Y_vMEutgdF12nqb" xr:uid="{FA4BDA58-B1DD-48D8-9C29-B4B1FADE61A0}"/>
+    <hyperlink ref="D29" r:id="rId3" xr:uid="{3D062E1E-43EA-4195-A895-604550782F7A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
summary pending of latest question
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854B04B9-4154-4C78-8194-55914F745AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6230853-3299-400A-A7B6-BC3AE6029364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="79">
   <si>
     <t>Question</t>
   </si>
@@ -518,6 +518,12 @@
   </si>
   <si>
     <t>4. Median of Two Sorted Arrays</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>143. Reorder List</t>
   </si>
 </sst>
 </file>
@@ -904,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1258,6 +1264,14 @@
         <v>75</v>
       </c>
     </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D21" r:id="rId1" xr:uid="{35299F42-C228-43E2-B954-EFB9EDC93588}"/>

</xml_diff>

<commit_message>
did the 143. Reorder List
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6230853-3299-400A-A7B6-BC3AE6029364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1726C02E-4455-4B66-A42E-F14E43FE6B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="80">
   <si>
     <t>Question</t>
   </si>
@@ -524,6 +524,15 @@
   </si>
   <si>
     <t>143. Reorder List</t>
+  </si>
+  <si>
+    <t>See neetcode's vid for more clear explaination
+The solution uses 2 ptrs, s &amp; f (slow &amp; fast) the s ptr starts at head in the while() and changes s = s.next while the f ptr initializes f = head.next &amp; in loop f changes as: f = f.next.next
+when f reaches null the s will be at mid pt, after this use another while loop to reverse the links of nodes after "s", use 3 ptrs for this, curr, currNext, currNextNext. 
+after the links the are reversed, make s.next = null since now s.next points to a node which in turn poits to "s"
+end = curr since if(currNext=null) we end the loop, so curr points the last node before currNext
+use p = head &amp; now use a while(p!=s) traverse the LL and keep popping nodes off from the end attach them in given order
+after the loop is done p will be = s so terminate the LL by p.next = null</t>
   </si>
 </sst>
 </file>
@@ -912,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1264,12 +1273,15 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>78</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
19. Remove Nth Node From End of List
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1726C02E-4455-4B66-A42E-F14E43FE6B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDC35FE-05BF-40DA-A7B1-DE27ED2533BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="82">
   <si>
     <t>Question</t>
   </si>
@@ -533,6 +533,14 @@
 end = curr since if(currNext=null) we end the loop, so curr points the last node before currNext
 use p = head &amp; now use a while(p!=s) traverse the LL and keep popping nodes off from the end attach them in given order
 after the loop is done p will be = s so terminate the LL by p.next = null</t>
+  </si>
+  <si>
+    <t>19. Remove Nth Node From End of List</t>
+  </si>
+  <si>
+    <t>Use 2 ptrs L &amp; R, initialize both = head, use while loop to move R by "n-1" places to the right of L
+Initalize a prev = null
+Now move both using while(R.next!=null) since both will maintain a fixed distance, after the end of the loop L will point to the node to be deleted. The "prev" pointer points to the node before L. Using prev delete L</t>
   </si>
 </sst>
 </file>
@@ -919,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1284,6 +1292,17 @@
         <v>79</v>
       </c>
     </row>
+    <row r="31" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D21" r:id="rId1" xr:uid="{35299F42-C228-43E2-B954-EFB9EDC93588}"/>

</xml_diff>

<commit_message>
138. Copy List with Random Pointer
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDC35FE-05BF-40DA-A7B1-DE27ED2533BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64106304-A08C-4840-975C-EF99E79D27AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
   <si>
     <t>Question</t>
   </si>
@@ -541,6 +541,16 @@
     <t>Use 2 ptrs L &amp; R, initialize both = head, use while loop to move R by "n-1" places to the right of L
 Initalize a prev = null
 Now move both using while(R.next!=null) since both will maintain a fixed distance, after the end of the loop L will point to the node to be deleted. The "prev" pointer points to the node before L. Using prev delete L</t>
+  </si>
+  <si>
+    <t>138. Copy List with Random Pointer</t>
+  </si>
+  <si>
+    <t>This is VERY TRICKY Problem, watch this video: https://youtu.be/5Y2EiZST97Y?si=Hxezj_ZugvAcGz3O
+The trick is to use a HashMap&lt;Node,Node&gt; we store mapping of oldNode, newNode in it. 
+first oldNode = head then use while(oldNode!=null) to iter over original LL, make new copy of each node with same val, leave the .random ptr as null. While creating new copies in the loop do hashmap.put(oldNode, newNode).... be sure to store new head of copy LL too
+Now we need to do a 2nd pass over original LL oldNode = head, using while(oldNode!=null) do newNode = hashmap.get(oldNode); newNode.random = hm.get(oldNode.random) || null; 
+USING HASHMAP FOR MAPPING OLDNODE: NEWNODE IS EXTREMLY IMPORTANT!!!!!!!</t>
   </si>
 </sst>
 </file>
@@ -927,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1303,6 +1313,17 @@
         <v>81</v>
       </c>
     </row>
+    <row r="32" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D21" r:id="rId1" xr:uid="{35299F42-C228-43E2-B954-EFB9EDC93588}"/>

</xml_diff>

<commit_message>
235. Lowest Common Ancestor of a Binary Search Tree
</commit_message>
<xml_diff>
--- a/Summary.xlsx
+++ b/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Folders to backup!!!\Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B30922F-B519-45C6-8EE2-48B02E9D2648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EF00C8-47E3-4DE1-A0E5-EDD71C240DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="120">
   <si>
     <t>Question</t>
   </si>
@@ -715,6 +715,25 @@
   <si>
     <t>This question is of DP &amp; extremly hard
 [https://youtu.be/HAA8mgxlov8?si=Zu3uuQ2Ax4ajpxRk]</t>
+  </si>
+  <si>
+    <t>235. Lowest Common Ancestor of a Binary Search Tree</t>
+  </si>
+  <si>
+    <t>We have to use **POSTORDER TRAVERSAL**. First recursively travel the tree in postorder. 
+After travelling the traversal function will return true of false if the subtree constains the given node. 
+boolean leftNode = postorder(node.left, p, q);
+boolean rightNode = postorder(node.right, p, q);
+now
+if both left &amp; right subtree contain the given nodes make a global variable LCA = current node ONLY if its NOT NULL &amp; then return true (due to the recursive nature of algo the first time both return true &amp; the LCA = current node ie Lowest common ansestor)
+else if either 1 of them is true (both cant be ture since we are checking that condition above) &amp;&amp; (q==currNode || p==currNode) make the global variable LCA = current node ONLY if its NOT NULL &amp; then return true (Lowest common decendant can be a decendent of itself)
+else if leftnode  or rightNode = true then return true // we have found a node atleast in the subtree below
+else{
+if(currNode = p or q) return true; // IMP CONDITION check of curr node is p or q
+else{return false} // this will only execute if p &amp; q are not in subtree below node
+}
+//base condition:
+if node=null return false</t>
   </si>
 </sst>
 </file>
@@ -812,7 +831,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -841,11 +860,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1128,10 +1144,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C52" sqref="C51:C52"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="102" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1676,15 +1692,29 @@
       <c r="A47" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="8" t="s">
         <v>117</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>116</v>
       </c>
+    </row>
+    <row r="48" spans="1:4" ht="360" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>